<commit_message>
#10 Excel file containing some incorrect Spanish URLs v2
</commit_message>
<xml_diff>
--- a/docs/spanish urls.xlsx
+++ b/docs/spanish urls.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="urls" sheetId="1" r:id="rId1"/>
+    <sheet name="spanish url" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="124">
   <si>
     <t>Here are some examples of mistakes in url domais (Spanish domains only):</t>
   </si>
@@ -208,13 +203,196 @@
   </si>
   <si>
     <t>lugo.gal</t>
+  </si>
+  <si>
+    <t>www.ava.es</t>
+  </si>
+  <si>
+    <t>ava.es</t>
+  </si>
+  <si>
+    <t>Probably related to Ayuntamiento de Valladolid</t>
+  </si>
+  <si>
+    <t>navalcarnero.es</t>
+  </si>
+  <si>
+    <t>www.navalcarnero.es</t>
+  </si>
+  <si>
+    <t>seu.selva.cat</t>
+  </si>
+  <si>
+    <t>www.selva.cat</t>
+  </si>
+  <si>
+    <t>www.aragon.es</t>
+  </si>
+  <si>
+    <t>servicios.aragon.es</t>
+  </si>
+  <si>
+    <t>contratacionpublica.aragon.es</t>
+  </si>
+  <si>
+    <t>www.ayuntamientoelcasar.es</t>
+  </si>
+  <si>
+    <t>elcasar.sedelectronica.es</t>
+  </si>
+  <si>
+    <t>www.sevilla.org</t>
+  </si>
+  <si>
+    <t>sevilla.org</t>
+  </si>
+  <si>
+    <t>www.dipusevilla.es</t>
+  </si>
+  <si>
+    <t>portal.dipusevilla.es</t>
+  </si>
+  <si>
+    <t>sedeelectronicadipusevilla.es</t>
+  </si>
+  <si>
+    <t>www.aytovillaviciosadeodon.es</t>
+  </si>
+  <si>
+    <t>sede.aytovillaviciosadeodon.es</t>
+  </si>
+  <si>
+    <t>perfilcontratante.red.es</t>
+  </si>
+  <si>
+    <t>perfilcontratacnte.red.es</t>
+  </si>
+  <si>
+    <t>perfilcontratante.res.es</t>
+  </si>
+  <si>
+    <t>www.ejie.eus</t>
+  </si>
+  <si>
+    <t>ataria.ejie.eus</t>
+  </si>
+  <si>
+    <t>www.ayto-arroyomolinos.org</t>
+  </si>
+  <si>
+    <t>www.arroyomolinos.org</t>
+  </si>
+  <si>
+    <t>The address in red belongs to a school</t>
+  </si>
+  <si>
+    <t>www.bilbaoport.es ; http</t>
+  </si>
+  <si>
+    <t>www.bilbaoport.es; http</t>
+  </si>
+  <si>
+    <t>www.bilbaoport.eus; http</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.bilbaoport.eus </t>
+  </si>
+  <si>
+    <t>www.bilbaoport.eus</t>
+  </si>
+  <si>
+    <t>www.bilbaoport.es</t>
+  </si>
+  <si>
+    <t>bilbao.eus</t>
+  </si>
+  <si>
+    <t>www.bilbao.eus</t>
+  </si>
+  <si>
+    <t>www.bilbao.net</t>
+  </si>
+  <si>
+    <t>www.contratacion.euskadi.es</t>
+  </si>
+  <si>
+    <t>www.osakidetza.euskadi.eus</t>
+  </si>
+  <si>
+    <t>www.osakidetza.euskadi.net</t>
+  </si>
+  <si>
+    <t>apps.euskadi.eus</t>
+  </si>
+  <si>
+    <t>www.euskadi.eus</t>
+  </si>
+  <si>
+    <t>contratacion.enaire.es</t>
+  </si>
+  <si>
+    <t>www.enaire.is</t>
+  </si>
+  <si>
+    <t>www.enaire.es</t>
+  </si>
+  <si>
+    <t>www.madird.org</t>
+  </si>
+  <si>
+    <t>vvww.aena-aeropuertos.es</t>
+  </si>
+  <si>
+    <t>wvvw.aena.es</t>
+  </si>
+  <si>
+    <t>wwvv.aena.es</t>
+  </si>
+  <si>
+    <t>contratacionnav.aena.es</t>
+  </si>
+  <si>
+    <t>wvvw.aena-aeropuertos.es</t>
+  </si>
+  <si>
+    <t>www.aena-aeropueitos.es</t>
+  </si>
+  <si>
+    <t>vww.aena-aeropuertos.es</t>
+  </si>
+  <si>
+    <t>vwvv.aena-aeropuertos.es</t>
+  </si>
+  <si>
+    <t>wwvv.aena-aeropuertos.es</t>
+  </si>
+  <si>
+    <t>vvvvw.aena.es</t>
+  </si>
+  <si>
+    <t>vvww.aena.es</t>
+  </si>
+  <si>
+    <t>xvww.aena.es</t>
+  </si>
+  <si>
+    <t>www. aena.es</t>
+  </si>
+  <si>
+    <t>www.aena.es</t>
+  </si>
+  <si>
+    <t>vww.aena.es</t>
+  </si>
+  <si>
+    <t>vvwvv.aena.es</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,6 +410,12 @@
     <font>
       <sz val="11"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -272,18 +456,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -296,7 +484,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -306,44 +494,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -371,14 +559,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -406,6 +611,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -417,182 +639,213 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K25"/>
+  <dimension ref="A2:R87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="30.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="30.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="12" max="17" width="30.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -605,14 +858,9 @@
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -625,14 +873,9 @@
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -642,15 +885,9 @@
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -660,15 +897,9 @@
       <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -681,33 +912,21 @@
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>6</v>
       </c>
       <c r="B13" s="4">
         <v>212142139196</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" t="s">
+      <c r="K13" s="1"/>
+      <c r="R13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -717,15 +936,9 @@
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -756,8 +969,9 @@
       <c r="J15" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>9</v>
       </c>
@@ -782,10 +996,9 @@
       <c r="H16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -795,15 +1008,9 @@
       <c r="C17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>11</v>
       </c>
@@ -813,15 +1020,9 @@
       <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -849,12 +1050,12 @@
       <c r="I19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" t="s">
+      <c r="K19" s="1"/>
+      <c r="R19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -864,15 +1065,9 @@
       <c r="C20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>14</v>
       </c>
@@ -882,18 +1077,12 @@
       <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" t="s">
+      <c r="K21" s="1"/>
+      <c r="R21" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>15</v>
       </c>
@@ -906,14 +1095,9 @@
       <c r="D22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>16</v>
       </c>
@@ -923,15 +1107,9 @@
       <c r="C23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>17</v>
       </c>
@@ -941,15 +1119,12 @@
       <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>18</v>
       </c>
@@ -959,15 +1134,502 @@
       <c r="C25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>19</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="R26" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>20</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>21</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>22</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>23</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>24</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>25</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>27</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>28</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="R36" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>30</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>32</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="1"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>33</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K40" s="1"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>34</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" s="1"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>35</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K42" s="1"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>36</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="O43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>37</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K44" s="1"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="K45" s="1"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="2"/>
+      <c r="K46" s="1"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="2"/>
+      <c r="K48" s="1"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="2"/>
+      <c r="K49" s="1"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="2"/>
+      <c r="K50" s="1"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+      <c r="K51" s="1"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="2"/>
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="2"/>
+      <c r="K53" s="1"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="2"/>
+      <c r="K54" s="1"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="2"/>
+      <c r="K55" s="1"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="2"/>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="2"/>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="2"/>
+      <c r="K58" s="1"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+      <c r="K59" s="1"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="2"/>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+      <c r="K61" s="1"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="2"/>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="2"/>
+      <c r="K65" s="1"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+      <c r="K66" s="1"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="2"/>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="2"/>
+      <c r="K68" s="1"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="2"/>
+      <c r="K69" s="1"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="2"/>
+      <c r="K70" s="1"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="2"/>
+      <c r="K71" s="1"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="2"/>
+      <c r="K72" s="1"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="2"/>
+      <c r="K73" s="1"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="2"/>
+      <c r="K74" s="1"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="2"/>
+      <c r="K75" s="1"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="K76" s="1"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="K77" s="1"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="K78" s="1"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="K79" s="1"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+      <c r="K80" s="1"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="K81" s="1"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="2"/>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+      <c r="K83" s="1"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="2"/>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" s="2"/>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" s="2"/>
+      <c r="K87" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>